<commit_message>
adding ncbr comp workbook from usproj
</commit_message>
<xml_diff>
--- a/data-raw/ncbr_comparison/BR_voluntarysupplement_2023.xlsx
+++ b/data-raw/ncbr_comparison/BR_voluntarysupplement_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\BTR\data-raw\model-runs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\BTR\data-raw\ncbr_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9640FAD-8C21-466D-874E-BAC580D994F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FD525D-1A52-48F6-B69A-FB2F908E50B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{5D257420-CEFD-4359-9AD1-E1CEE4FC7F7A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D257420-CEFD-4359-9AD1-E1CEE4FC7F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="br_vs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="44">
   <si>
     <t>source</t>
   </si>
@@ -65,85 +65,43 @@
     <t>Mt CO2e/yr</t>
   </si>
   <si>
-    <t>GHGI 2024</t>
-  </si>
-  <si>
     <t>N2O</t>
-  </si>
-  <si>
-    <t>GHGI 2025</t>
   </si>
   <si>
     <t>HFCs</t>
   </si>
   <si>
-    <t>GHGI 2026</t>
-  </si>
-  <si>
     <t>PFCs</t>
-  </si>
-  <si>
-    <t>GHGI 2027</t>
   </si>
   <si>
     <t>SF6</t>
   </si>
   <si>
-    <t>GHGI 2028</t>
-  </si>
-  <si>
     <t>NF3</t>
-  </si>
-  <si>
-    <t>GHGI 2029</t>
   </si>
   <si>
     <t>Total Gross Emissions</t>
   </si>
   <si>
-    <t>GHGI 2030</t>
-  </si>
-  <si>
     <t>LULUCF</t>
-  </si>
-  <si>
-    <t>GHGI 2031</t>
   </si>
   <si>
     <t>Total Net Emissions</t>
   </si>
   <si>
-    <t>GHGI 2032</t>
-  </si>
-  <si>
     <t>Energy</t>
-  </si>
-  <si>
-    <t>GHGI 2033</t>
   </si>
   <si>
     <t>Transportation</t>
   </si>
   <si>
-    <t>GHGI 2034</t>
-  </si>
-  <si>
     <t>Industrial Processes</t>
-  </si>
-  <si>
-    <t>GHGI 2035</t>
   </si>
   <si>
     <t>Agriculture</t>
   </si>
   <si>
-    <t>GHGI 2036</t>
-  </si>
-  <si>
     <t>Waste</t>
-  </si>
-  <si>
-    <t>GHGI 2037</t>
   </si>
   <si>
     <t>BR5</t>
@@ -569,38 +527,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1B0D53-9ADE-48A6-BC42-2754A1B685E6}">
   <dimension ref="A1:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67:M80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1">
         <v>2005</v>
@@ -630,15 +588,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -656,21 +614,21 @@
         <v>4737</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -688,24 +646,24 @@
         <v>729.12</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -720,24 +678,24 @@
         <v>364.59731543624156</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -752,24 +710,24 @@
         <v>123.83</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -788,24 +746,24 @@
         <v>5</v>
       </c>
       <c r="M6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -820,24 +778,24 @@
         <v>4.1228070175438596</v>
       </c>
       <c r="M7" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -852,24 +810,24 @@
         <v>0.93604651162790697</v>
       </c>
       <c r="M8" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -884,24 +842,24 @@
         <v>5964.6061689654134</v>
       </c>
       <c r="M9" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -916,24 +874,24 @@
         <v>-724</v>
       </c>
       <c r="M10" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -948,24 +906,24 @@
         <v>5240.6061689654134</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -980,24 +938,24 @@
         <v>3191.3305354593995</v>
       </c>
       <c r="M12" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1012,24 +970,24 @@
         <v>1697.4225665950578</v>
       </c>
       <c r="M13" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1044,24 +1002,24 @@
         <v>354.10204126030436</v>
       </c>
       <c r="M14" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1076,24 +1034,24 @@
         <v>562.66851986659947</v>
       </c>
       <c r="M15" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1108,24 +1066,24 @@
         <v>159.17658177801141</v>
       </c>
       <c r="M16" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -1140,24 +1098,24 @@
         <v>-846</v>
       </c>
       <c r="M17" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1172,24 +1130,24 @@
         <v>5118.6061689654134</v>
       </c>
       <c r="M18" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="N18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
@@ -1204,24 +1162,24 @@
         <v>-602</v>
       </c>
       <c r="M19" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="N19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1236,21 +1194,21 @@
         <v>5362.6061689654134</v>
       </c>
       <c r="M20" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -1268,15 +1226,15 @@
         <v>3037.8479879999991</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -1294,18 +1252,18 @@
         <v>728.80697176560011</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1320,18 +1278,18 @@
         <v>397.06839792379998</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1346,18 +1304,18 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1372,18 +1330,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1398,18 +1356,18 @@
         <v>4.1228070175438596</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1424,18 +1382,18 @@
         <v>0.93604651162790697</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -1450,18 +1408,18 @@
         <v>4297.6122112185712</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -1476,18 +1434,18 @@
         <v>-708.38831999999991</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -1502,18 +1460,18 @@
         <v>3589.2238912185712</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -1528,18 +1486,18 @@
         <v>2299.4143604294263</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
@@ -1554,18 +1512,18 @@
         <v>1223.0252498065961</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1580,18 +1538,18 @@
         <v>255.13725691660676</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1606,18 +1564,18 @@
         <v>405.41337237466132</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1632,15 +1590,15 @@
         <v>114.68975523456393</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -1658,15 +1616,15 @@
         <v>3265</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -1684,18 +1642,18 @@
         <v>688</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -1710,18 +1668,18 @@
         <v>364.59731543624156</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -1736,18 +1694,18 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
@@ -1762,18 +1720,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1788,18 +1746,18 @@
         <v>4.1228070175438596</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
@@ -1814,18 +1772,18 @@
         <v>0.93604651162790697</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
@@ -1840,18 +1798,18 @@
         <v>4451.4861689654135</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
         <v>5</v>
@@ -1866,18 +1824,18 @@
         <v>-751.71753902945318</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1892,18 +1850,18 @@
         <v>3699.7686299359602</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -1918,18 +1876,18 @@
         <v>2381.7437961136375</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1944,18 +1902,18 @@
         <v>1266.8150862001175</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D48" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -1970,18 +1928,18 @@
         <v>264.27232484757292</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D49" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
@@ -1996,18 +1954,18 @@
         <v>419.92900502479637</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D50" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
@@ -2022,15 +1980,15 @@
         <v>118.79616728004605</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
@@ -2048,15 +2006,15 @@
         <v>3310.1080503108101</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -2074,18 +2032,18 @@
         <v>689.90849353400802</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
@@ -2100,18 +2058,18 @@
         <v>364.59731543624156</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
@@ -2126,18 +2084,18 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
@@ -2152,18 +2110,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
@@ -2178,18 +2136,18 @@
         <v>4.1228070175438596</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D57" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E57" t="s">
         <v>8</v>
@@ -2204,18 +2162,18 @@
         <v>0.93604651162790697</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D58" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
@@ -2230,18 +2188,18 @@
         <v>4498.5027128102311</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D59" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E59" t="s">
         <v>5</v>
@@ -2256,18 +2214,18 @@
         <v>-841.85541836975301</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D60" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E60" t="s">
         <v>8</v>
@@ -2282,18 +2240,18 @@
         <v>3656.6472944404782</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C61" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D61" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
@@ -2308,18 +2266,18 @@
         <v>2406.8997456924103</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D62" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E62" t="s">
         <v>8</v>
@@ -2334,18 +2292,18 @@
         <v>1280.1951720372588</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C63" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D63" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E63" t="s">
         <v>8</v>
@@ -2360,18 +2318,18 @@
         <v>267.06356599188842</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C64" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D64" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E64" t="s">
         <v>8</v>
@@ -2386,18 +2344,18 @@
         <v>424.36429016936364</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D65" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E65" t="s">
         <v>8</v>
@@ -2412,7 +2370,7 @@
         <v>120.05089098253858</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -2420,7 +2378,7 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D66" t="s">
         <v>4</v>
@@ -2444,7 +2402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -2452,7 +2410,7 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -2473,10 +2431,10 @@
         <v>727.4</v>
       </c>
       <c r="M67" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -2484,10 +2442,10 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
@@ -2505,10 +2463,10 @@
         <v>393.3</v>
       </c>
       <c r="M68" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -2516,10 +2474,10 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E69" t="s">
         <v>8</v>
@@ -2537,10 +2495,10 @@
         <v>175.1</v>
       </c>
       <c r="M69" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -2548,10 +2506,10 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -2569,10 +2527,10 @@
         <v>3.5</v>
       </c>
       <c r="M70" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -2580,10 +2538,10 @@
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D71" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E71" t="s">
         <v>8</v>
@@ -2601,10 +2559,10 @@
         <v>8</v>
       </c>
       <c r="M71" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -2612,10 +2570,10 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D72" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2633,10 +2591,10 @@
         <v>0.6</v>
       </c>
       <c r="M72" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -2644,10 +2602,10 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D73" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -2665,10 +2623,10 @@
         <v>6340.2</v>
       </c>
       <c r="M73" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -2676,10 +2634,10 @@
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D74" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E74" t="s">
         <v>5</v>
@@ -2697,10 +2655,10 @@
         <v>-754.2</v>
       </c>
       <c r="M74" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -2708,10 +2666,10 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D75" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E75" t="s">
         <v>8</v>
@@ -2729,10 +2687,10 @@
         <v>5586</v>
       </c>
       <c r="M75" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -2740,10 +2698,10 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D76" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
@@ -2761,10 +2719,10 @@
         <v>3392.2900000000004</v>
       </c>
       <c r="M76" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -2772,10 +2730,10 @@
         <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D77" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
@@ -2793,10 +2751,10 @@
         <v>1804.31</v>
       </c>
       <c r="M77" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -2804,10 +2762,10 @@
         <v>3</v>
       </c>
       <c r="C78" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D78" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E78" t="s">
         <v>8</v>
@@ -2825,10 +2783,10 @@
         <v>376.4</v>
       </c>
       <c r="M78" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -2836,10 +2794,10 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D79" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E79" t="s">
         <v>8</v>
@@ -2857,10 +2815,10 @@
         <v>598.1</v>
       </c>
       <c r="M79" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -2868,10 +2826,10 @@
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D80" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2889,18 +2847,18 @@
         <v>169.2</v>
       </c>
       <c r="M80" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B81" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C81" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D81" t="s">
         <v>4</v>
@@ -2918,15 +2876,15 @@
         <v>3385.68</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B82" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C82" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -2944,18 +2902,18 @@
         <v>729.12</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B83" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C83" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
@@ -2970,18 +2928,18 @@
         <v>364.59731543624156</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B84" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D84" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2996,18 +2954,18 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C85" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D85" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
@@ -3022,18 +2980,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D86" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E86" t="s">
         <v>8</v>
@@ -3048,18 +3006,18 @@
         <v>4.1228070175438596</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C87" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D87" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E87" t="s">
         <v>8</v>
@@ -3074,18 +3032,18 @@
         <v>0.93604651162790697</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D88" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E88" t="s">
         <v>8</v>
@@ -3100,18 +3058,18 @@
         <v>4613.2861689654137</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C89" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D89" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E89" t="s">
         <v>5</v>
@@ -3126,18 +3084,18 @@
         <v>-755.05</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C90" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D90" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E90" t="s">
         <v>8</v>
@@ -3152,18 +3110,18 @@
         <v>3858.2361689654135</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D91" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
@@ -3178,18 +3136,18 @@
         <v>2468.3140181886511</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C92" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D92" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E92" t="s">
         <v>8</v>
@@ -3204,18 +3162,18 @@
         <v>1312.8605355550276</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D93" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E93" t="s">
         <v>8</v>
@@ -3230,18 +3188,18 @@
         <v>273.87793981240054</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C94" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D94" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E94" t="s">
         <v>8</v>
@@ -3256,18 +3214,18 @@
         <v>435.19233741178732</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C95" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D95" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E95" t="s">
         <v>8</v>
@@ -3282,15 +3240,15 @@
         <v>123.11410046827355</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D96" t="s">
         <v>4</v>
@@ -3308,15 +3266,15 @@
         <v>3347.49847</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C97" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D97" t="s">
         <v>7</v>
@@ -3334,18 +3292,18 @@
         <v>729.12</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C98" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E98" t="s">
         <v>8</v>
@@ -3360,18 +3318,18 @@
         <v>364.59731543624156</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B99" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C99" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D99" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E99" t="s">
         <v>8</v>
@@ -3386,18 +3344,18 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C100" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D100" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E100" t="s">
         <v>8</v>
@@ -3412,18 +3370,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B101" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C101" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D101" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E101" t="s">
         <v>8</v>
@@ -3438,18 +3396,18 @@
         <v>4.1228070175438596</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B102" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C102" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D102" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E102" t="s">
         <v>8</v>
@@ -3464,18 +3422,18 @@
         <v>0.93604651162790697</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C103" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D103" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E103" t="s">
         <v>8</v>
@@ -3490,18 +3448,18 @@
         <v>4575.104638965413</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B104" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C104" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D104" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E104" t="s">
         <v>5</v>
@@ -3516,18 +3474,18 @@
         <v>-724</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B105" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C105" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D105" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E105" t="s">
         <v>8</v>
@@ -3542,18 +3500,18 @@
         <v>3851.104638965413</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C106" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D106" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E106" t="s">
         <v>8</v>
@@ -3568,18 +3526,18 @@
         <v>2447.8851953749063</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B107" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C107" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D107" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E107" t="s">
         <v>8</v>
@@ -3594,18 +3552,18 @@
         <v>1301.994740092061</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B108" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C108" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D108" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E108" t="s">
         <v>8</v>
@@ -3620,18 +3578,18 @@
         <v>271.61120881148565</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B109" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C109" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D109" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E109" t="s">
         <v>8</v>
@@ -3646,18 +3604,18 @@
         <v>431.59049944248034</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B110" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C110" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D110" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E110" t="s">
         <v>8</v>
@@ -3672,15 +3630,15 @@
         <v>122.09515550186869</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B111" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C111" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D111" t="s">
         <v>4</v>
@@ -3698,15 +3656,15 @@
         <v>3572.5756357527198</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B112" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C112" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D112" t="s">
         <v>7</v>
@@ -3724,18 +3682,18 @@
         <v>636.60599204717596</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B113" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C113" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D113" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E113" t="s">
         <v>8</v>
@@ -3750,18 +3708,18 @@
         <v>381.37707135344601</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B114" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C114" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D114" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E114" t="s">
         <v>8</v>
@@ -3776,18 +3734,18 @@
         <v>83.090833837750594</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B115" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C115" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D115" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E115" t="s">
         <v>8</v>
@@ -3802,18 +3760,18 @@
         <v>5.1056099149243597</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B116" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C116" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D116" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E116" t="s">
         <v>8</v>
@@ -3828,18 +3786,18 @@
         <v>5.3261829961328804</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B117" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C117" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D117" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E117" t="s">
         <v>8</v>
@@ -3854,18 +3812,18 @@
         <v>0.76217412256737405</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B118" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C118" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D118" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E118" t="s">
         <v>8</v>
@@ -3880,18 +3838,18 @@
         <v>4684.8435000247173</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B119" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C119" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D119" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E119" t="s">
         <v>5</v>
@@ -3906,18 +3864,18 @@
         <v>-903.30680465987098</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B120" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C120" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D120" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E120" t="s">
         <v>8</v>
@@ -3932,18 +3890,18 @@
         <v>3781.5366953648463</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B121" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C121" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D121" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E121" t="s">
         <v>8</v>
@@ -3958,18 +3916,18 @@
         <v>2332.54705151086</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B122" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C122" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D122" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E122" t="s">
         <v>8</v>
@@ -3984,18 +3942,18 @@
         <v>1346.0420396172699</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B123" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C123" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D123" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E123" t="s">
         <v>8</v>
@@ -4010,18 +3968,18 @@
         <v>274.55905739844201</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B124" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C124" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D124" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E124" t="s">
         <v>8</v>
@@ -4036,18 +3994,18 @@
         <v>592.10472791789402</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B125" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C125" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D125" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E125" t="s">
         <v>8</v>
@@ -4062,15 +4020,15 @@
         <v>139.59062358025699</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B126" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C126" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D126" t="s">
         <v>4</v>
@@ -4088,15 +4046,15 @@
         <v>3158.1921519295602</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C127" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D127" t="s">
         <v>7</v>
@@ -4114,18 +4072,18 @@
         <v>729.12</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C128" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E128" t="s">
         <v>8</v>
@@ -4140,18 +4098,18 @@
         <v>364.59731543624156</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B129" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C129" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D129" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E129" t="s">
         <v>8</v>
@@ -4166,18 +4124,18 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B130" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C130" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D130" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E130" t="s">
         <v>8</v>
@@ -4192,18 +4150,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C131" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D131" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E131" t="s">
         <v>8</v>
@@ -4218,18 +4176,18 @@
         <v>4.1228070175438596</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C132" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D132" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E132" t="s">
         <v>8</v>
@@ -4244,18 +4202,18 @@
         <v>0.93604651162790697</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C133" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D133" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -4270,18 +4228,18 @@
         <v>4385.7983208949736</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C134" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D134" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E134" t="s">
         <v>5</v>
@@ -4296,18 +4254,18 @@
         <v>-724</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C135" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D135" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E135" t="s">
         <v>8</v>
@@ -4322,18 +4280,18 @@
         <v>3661.7983208949736</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B136" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C136" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D136" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E136" t="s">
         <v>8</v>
@@ -4348,18 +4306,18 @@
         <v>2346.5978653652583</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C137" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D137" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E137" t="s">
         <v>8</v>
@@ -4374,18 +4332,18 @@
         <v>1248.1214738295339</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C138" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D138" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E138" t="s">
         <v>8</v>
@@ -4400,18 +4358,18 @@
         <v>260.37262041968205</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C139" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D139" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E139" t="s">
         <v>8</v>
@@ -4426,18 +4384,18 @@
         <v>413.73237054466483</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C140" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D140" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E140" t="s">
         <v>8</v>
@@ -4452,15 +4410,15 @@
         <v>117.04316518334272</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B141" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C141" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D141" t="s">
         <v>4</v>
@@ -4478,15 +4436,15 @@
         <v>2763</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B142" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C142" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D142" t="s">
         <v>7</v>
@@ -4504,18 +4462,18 @@
         <v>729.12</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B143" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C143" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D143" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E143" t="s">
         <v>8</v>
@@ -4530,18 +4488,18 @@
         <v>364.59731543624156</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B144" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C144" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D144" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E144" t="s">
         <v>8</v>
@@ -4556,18 +4514,18 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B145" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C145" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D145" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E145" t="s">
         <v>8</v>
@@ -4582,18 +4540,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B146" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C146" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D146" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E146" t="s">
         <v>8</v>
@@ -4608,18 +4566,18 @@
         <v>4.1228070175438596</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C147" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D147" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E147" t="s">
         <v>8</v>
@@ -4634,18 +4592,18 @@
         <v>0.93604651162790697</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B148" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C148" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D148" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E148" t="s">
         <v>8</v>
@@ -4660,18 +4618,18 @@
         <v>3990.606168965413</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B149" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C149" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D149" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E149" t="s">
         <v>5</v>
@@ -4686,18 +4644,18 @@
         <v>-646.13446706911805</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B150" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C150" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D150" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E150" t="s">
         <v>8</v>
@@ -4712,18 +4670,18 @@
         <v>3344.4717018962947</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B151" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C151" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D151" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E151" t="s">
         <v>8</v>
@@ -4738,18 +4696,18 @@
         <v>2135.1524243588028</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B152" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C152" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D152" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E152" t="s">
         <v>8</v>
@@ -4764,18 +4722,18 @@
         <v>1135.6567011649452</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B153" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C153" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D153" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E153" t="s">
         <v>8</v>
@@ -4790,18 +4748,18 @@
         <v>236.91116400091187</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B154" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C154" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D154" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E154" t="s">
         <v>8</v>
@@ -4816,18 +4774,18 @@
         <v>376.45209136276674</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B155" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C155" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D155" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E155" t="s">
         <v>8</v>
@@ -4842,15 +4800,15 @@
         <v>106.49672940742371</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B156" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C156" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D156" t="s">
         <v>4</v>
@@ -4868,15 +4826,15 @@
         <v>3231.66939</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B157" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C157" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D157" t="s">
         <v>7</v>
@@ -4894,18 +4852,18 @@
         <v>729.12</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B158" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C158" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D158" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E158" t="s">
         <v>8</v>
@@ -4920,18 +4878,18 @@
         <v>364.59731543624156</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B159" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C159" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D159" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E159" t="s">
         <v>8</v>
@@ -4946,18 +4904,18 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B160" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C160" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D160" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E160" t="s">
         <v>8</v>
@@ -4972,18 +4930,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B161" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C161" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D161" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E161" t="s">
         <v>8</v>
@@ -4998,18 +4956,18 @@
         <v>4.1228070175438596</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B162" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C162" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D162" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E162" t="s">
         <v>8</v>
@@ -5024,18 +4982,18 @@
         <v>0.93604651162790697</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B163" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C163" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D163" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E163" t="s">
         <v>8</v>
@@ -5050,18 +5008,18 @@
         <v>4459.2755589654134</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B164" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C164" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D164" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E164" t="s">
         <v>5</v>
@@ -5076,18 +5034,18 @@
         <v>-724</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B165" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C165" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D165" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E165" t="s">
         <v>8</v>
@@ -5102,18 +5060,18 @@
         <v>3735.2755589654134</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B166" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C166" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D166" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E166" t="s">
         <v>8</v>
@@ -5128,18 +5086,18 @@
         <v>2385.9114674494153</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B167" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C167" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D167" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E167" t="s">
         <v>8</v>
@@ -5154,18 +5112,18 @@
         <v>1269.0318103209497</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B168" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C168" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D168" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E168" t="s">
         <v>8</v>
@@ -5180,18 +5138,18 @@
         <v>264.73475921809745</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B169" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C169" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D169" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E169" t="s">
         <v>8</v>
@@ -5206,18 +5164,18 @@
         <v>420.66381373098858</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B170" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C170" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D170" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E170" t="s">
         <v>8</v>

</xml_diff>